<commit_message>
Fixes wrong X data for minutiae
Fixes X data for minutiae 21, with approximate value by checking the
image
</commit_message>
<xml_diff>
--- a/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-2-0.xlsx
+++ b/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-2-0.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Final Template" sheetId="3" r:id="rId2"/>
     <sheet name="Support Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -194,6 +194,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -206,7 +207,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,8 +490,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C2">
@@ -594,25 +594,25 @@
         <f>CONCATENATE(I2,J2,'Support Data'!$C$7,K2,L2,'Support Data'!$C$8)</f>
         <v>809900111200</v>
       </c>
-      <c r="P2" s="13" t="str">
+      <c r="P2" s="14" t="str">
         <f>CONCATENATE('Support Data'!D11,'Support Data'!D12,'Support Data'!D13,'Support Data'!D14)</f>
         <v>464D520020323000000000AE0000012C019000C500C5010000105B18</v>
       </c>
-      <c r="Q2" s="14" t="e">
+      <c r="Q2" s="15" t="str">
         <f>CONCATENATE(P2,P10,'Support Data'!C17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
+        <v>464D520020323000000000AE0000012C019000C500C5010000105B18809900111200407A0031920080AC002E0C00809200450A0080B5003A8D0040E80055830040EB006C0100403E00B5A20040BA00848500404700D71E00806900E21D0040FB00AA7300403201481E00409B012A2000404A015E1A004051016A1400407901701700809A01599E0080850173140040FA0156600080FE0148530080F00163670080C701550E0080F2018569000000</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C3">
@@ -648,19 +648,19 @@
         <f>CONCATENATE(I3,J3,'Support Data'!$C$7,K3,L3,'Support Data'!$C$8)</f>
         <v>407A00319200</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -696,18 +696,18 @@
         <f>CONCATENATE(I4,J4,'Support Data'!$C$7,K4,L4,'Support Data'!$C$8)</f>
         <v>80AC002E0C00</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C5">
@@ -743,18 +743,18 @@
         <f>CONCATENATE(I5,J5,'Support Data'!$C$7,K5,L5,'Support Data'!$C$8)</f>
         <v>809200450A00</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C6">
@@ -795,7 +795,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C7">
@@ -836,7 +836,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C8">
@@ -877,7 +877,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C9">
@@ -921,7 +921,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C10">
@@ -957,16 +957,16 @@
         <f>CONCATENATE(I10,J10,'Support Data'!$C$7,K10,L10,'Support Data'!$C$8)</f>
         <v>40BA00848500</v>
       </c>
-      <c r="P10" s="1" t="e">
+      <c r="P10" s="1" t="str">
         <f>CONCATENATE(M2,M3,M4,M5,M6,M7,M8,M9,M10,M11,M12,M13,M14,M15,M16,M17,M18,M19,M20,M21,M22,M23,M24,M25,M26,M27,M28,M29,M30,M31,M32,M33,M34,M35,M36,M37,M38,M39,M40,M41,M42,M43,M44,M45,M46,M47,M48,M49,M50,M51,M52,M53,M54,M55,M56,M57,M58,M59,M60,M61,M62,M63,M64,M65,M66,M67,M68,M69,M70,M71,M72,M73,M74,M75,M76,M77,M78,M79,M80,M81,M82,M83,M84,M85,M86,M87,M88,M89,M90,M91,M92,M93,M94,M95,M96,M97,M98,M99,M100,M101,M102,M103,M104,M105,M106,M107,M108,M109,M110,M111,M112,M113,M114,M115,M116,M117,M118,M119,M120,M121,M122,M123,M124,M125,M126,M127,M128,M129,M130,M131,M132,M133,M134,M135,M136,M137,M138,M139,M140,M141,M142,M143,M144,M145,M146,M147,M148,M149,M150)</f>
-        <v>#NUM!</v>
+        <v>809900111200407A0031920080AC002E0C00809200450A0080B5003A8D0040E80055830040EB006C0100403E00B5A20040BA00848500404700D71E00806900E21D0040FB00AA7300403201481E00409B012A2000404A015E1A004051016A1400407901701700809A01599E0080850173140040FA0156600080FE0148530080F00163670080C701550E0080F201856900</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -1007,7 +1007,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C12">
@@ -1048,7 +1048,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C13">
@@ -1089,7 +1089,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C14">
@@ -1130,7 +1130,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C15">
@@ -1171,7 +1171,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1212,7 +1212,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C17">
@@ -1253,7 +1253,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C18">
@@ -1294,7 +1294,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C19">
@@ -1335,7 +1335,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C20">
@@ -1376,7 +1376,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C21">
@@ -1417,11 +1417,11 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="12">
-        <v>274.286</v>
+        <v>254.286</v>
       </c>
       <c r="D22">
         <v>328.57100000000003</v>
@@ -1437,9 +1437,9 @@
         <f>IF(B22='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
         <v>80</v>
       </c>
-      <c r="J22" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>FE</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
@@ -1449,16 +1449,16 @@
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="M22" t="e">
+      <c r="M22" t="str">
         <f>CONCATENATE(I22,J22,'Support Data'!$C$7,K22,L22,'Support Data'!$C$8)</f>
-        <v>#NUM!</v>
+        <v>80FE01485300</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C23">
@@ -1499,7 +1499,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C24">
@@ -1540,7 +1540,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C25">
@@ -1604,9 +1604,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>'Collected Minutiae'!Q2</f>
-        <v>#NUM!</v>
+        <v>464D520020323000000000AE0000012C019000C500C5010000105B18809900111200407A0031920080AC002E0C00809200450A0080B5003A8D0040E80055830040EB006C0100403E00B5A20040BA00848500404700D71E00806900E21D0040FB00AA7300403201481E00409B012A2000404A015E1A004051016A1400407901701700809A01599E0080850173140040FA0156600080FE0148530080F00163670080C701550E0080F2018569000000</v>
       </c>
     </row>
   </sheetData>
@@ -1630,15 +1630,15 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1733,10 +1733,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="17"/>
       <c r="D11" t="s">
         <v>22</v>
       </c>
@@ -1768,10 +1768,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="1" t="str">
         <f>DEC2HEX(COUNT('Collected Minutiae'!A2:A1000), 2)</f>
         <v>18</v>

</xml_diff>